<commit_message>
management added. update README
</commit_message>
<xml_diff>
--- a/database/Management/MGM_Programs.xlsx
+++ b/database/Management/MGM_Programs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\OneDrive\20110706\TaiGer_Transcript-Program_Comparer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c520cbcd5c1ba828/20110706/TaiGer_Transcript-Program_Comparer/database/Management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414A81D0-BF80-4590-992B-60A89E3DD0FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{414A81D0-BF80-4590-992B-60A89E3DD0FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58A9AE49-1D84-401D-94E0-2AEF4E3E329B}"/>
   <bookViews>
-    <workbookView xWindow="21825" yWindow="-16350" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6975" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Program_choosing" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>Program</t>
   </si>
@@ -36,19 +36,13 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>RWTH Aachen AUTO</t>
-  </si>
-  <si>
-    <t>TUHH_MECHATRONICS</t>
-  </si>
-  <si>
-    <t>HANNOVER_INTER_MECHATRONICS</t>
-  </si>
-  <si>
-    <t>TU_DORTMUND_MANUFACTURING_TECH</t>
-  </si>
-  <si>
-    <t>TUM_MW</t>
+    <t>TUM_MMT</t>
+  </si>
+  <si>
+    <t>TUM_Consumer_Science</t>
+  </si>
+  <si>
+    <t>Uni_Koeln_BA</t>
   </si>
 </sst>
 </file>
@@ -366,15 +360,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="1" max="1" width="32" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -395,7 +389,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -403,25 +397,9 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add 3 programs in MGM.
</commit_message>
<xml_diff>
--- a/database/Management/MGM_Programs.xlsx
+++ b/database/Management/MGM_Programs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c520cbcd5c1ba828/20110706/TaiGer_Transcript-Program_Comparer/database/Management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{414A81D0-BF80-4590-992B-60A89E3DD0FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58A9AE49-1D84-401D-94E0-2AEF4E3E329B}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{414A81D0-BF80-4590-992B-60A89E3DD0FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DFAF9483-5804-47AF-A14E-037817C22FDF}"/>
   <bookViews>
-    <workbookView xWindow="-6975" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21825" yWindow="-16350" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Program_choosing" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>Program</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>Uni_Koeln_BA</t>
+  </si>
+  <si>
+    <t>Uni_Mannheim_MGM</t>
+  </si>
+  <si>
+    <t>Uni_Magdeburg_Finalcial_Economics</t>
   </si>
 </sst>
 </file>
@@ -360,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -403,6 +409,22 @@
         <v>2</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B6" xr:uid="{610A300D-EA49-404E-A3AA-32352271D928}">

</xml_diff>